<commit_message>
Implementación envío automático de diplomas por correo
</commit_message>
<xml_diff>
--- a/evidencias2020.xlsx
+++ b/evidencias2020.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\InnosoftDiploma\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3189A2-40F7-4EDC-AB67-A18C76FB61E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="4452" yWindow="2280" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
   <si>
     <t>D.N.I.</t>
   </si>
@@ -80,169 +96,170 @@
     <t>alumno1</t>
   </si>
   <si>
+    <t>http://evidentia.test/20/profiles/view/1</t>
+  </si>
+  <si>
+    <t>ASSISTANCE</t>
+  </si>
+  <si>
+    <t>Merino Verde</t>
+  </si>
+  <si>
+    <t>Enrique</t>
+  </si>
+  <si>
+    <t>alumno2</t>
+  </si>
+  <si>
+    <t>alumno2@alumno2.com</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/2</t>
+  </si>
+  <si>
+    <t>Biedma Fresno</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>secretario1</t>
+  </si>
+  <si>
+    <t>secretario1@secretario1.com</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/3</t>
+  </si>
+  <si>
+    <t>Sostenibilidad</t>
+  </si>
+  <si>
+    <t>Gata Fernández</t>
+  </si>
+  <si>
+    <t>José Manuel</t>
+  </si>
+  <si>
+    <t>secretario2</t>
+  </si>
+  <si>
+    <t>secretario2@secretario2.com</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/4</t>
+  </si>
+  <si>
+    <t>Logística</t>
+  </si>
+  <si>
+    <t>Hendricks</t>
+  </si>
+  <si>
+    <t>Margaret</t>
+  </si>
+  <si>
+    <t>coordinador1</t>
+  </si>
+  <si>
+    <t>coordinador1@coordinador1.com</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/5</t>
+  </si>
+  <si>
+    <t>Rowley</t>
+  </si>
+  <si>
+    <t>Diana</t>
+  </si>
+  <si>
+    <t>coordinador2</t>
+  </si>
+  <si>
+    <t>coordinador2@coordinador2.com</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/6</t>
+  </si>
+  <si>
+    <t>Clayton</t>
+  </si>
+  <si>
+    <t>Karl</t>
+  </si>
+  <si>
+    <t>coordinadorregistro1</t>
+  </si>
+  <si>
+    <t>coordinadorregistro1@coordinadorregistro1.com</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/7</t>
+  </si>
+  <si>
+    <t>Hart</t>
+  </si>
+  <si>
+    <t>Clara</t>
+  </si>
+  <si>
+    <t>coordinadorregistro2</t>
+  </si>
+  <si>
+    <t>coordinadorregistro2@coordinadorregistro2.com</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/8</t>
+  </si>
+  <si>
+    <t>Liu</t>
+  </si>
+  <si>
+    <t>Jamie-Leigh</t>
+  </si>
+  <si>
+    <t>presidente1</t>
+  </si>
+  <si>
+    <t>presidente1@presidente1.com</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/9</t>
+  </si>
+  <si>
+    <t>Alé</t>
+  </si>
+  <si>
+    <t>Francisco</t>
+  </si>
+  <si>
+    <t>presidente2</t>
+  </si>
+  <si>
+    <t>presidente2@presidente2.com</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/10</t>
+  </si>
+  <si>
     <t>alumno1@alumno1.com</t>
-  </si>
-  <si>
-    <t>http://evidentia.test/20/profiles/view/1</t>
-  </si>
-  <si>
-    <t>ASSISTANCE</t>
-  </si>
-  <si>
-    <t>Merino Verde</t>
-  </si>
-  <si>
-    <t>Enrique</t>
-  </si>
-  <si>
-    <t>alumno2</t>
-  </si>
-  <si>
-    <t>alumno2@alumno2.com</t>
-  </si>
-  <si>
-    <t>http://evidentia.test/20/profiles/view/2</t>
-  </si>
-  <si>
-    <t>Biedma Fresno</t>
-  </si>
-  <si>
-    <t>Pedro</t>
-  </si>
-  <si>
-    <t>secretario1</t>
-  </si>
-  <si>
-    <t>secretario1@secretario1.com</t>
-  </si>
-  <si>
-    <t>http://evidentia.test/20/profiles/view/3</t>
-  </si>
-  <si>
-    <t>Sostenibilidad</t>
-  </si>
-  <si>
-    <t>Gata Fernández</t>
-  </si>
-  <si>
-    <t>José Manuel</t>
-  </si>
-  <si>
-    <t>secretario2</t>
-  </si>
-  <si>
-    <t>secretario2@secretario2.com</t>
-  </si>
-  <si>
-    <t>http://evidentia.test/20/profiles/view/4</t>
-  </si>
-  <si>
-    <t>Logística</t>
-  </si>
-  <si>
-    <t>Hendricks</t>
-  </si>
-  <si>
-    <t>Margaret</t>
-  </si>
-  <si>
-    <t>coordinador1</t>
-  </si>
-  <si>
-    <t>coordinador1@coordinador1.com</t>
-  </si>
-  <si>
-    <t>http://evidentia.test/20/profiles/view/5</t>
-  </si>
-  <si>
-    <t>Rowley</t>
-  </si>
-  <si>
-    <t>Diana</t>
-  </si>
-  <si>
-    <t>coordinador2</t>
-  </si>
-  <si>
-    <t>coordinador2@coordinador2.com</t>
-  </si>
-  <si>
-    <t>http://evidentia.test/20/profiles/view/6</t>
-  </si>
-  <si>
-    <t>Clayton</t>
-  </si>
-  <si>
-    <t>Karl</t>
-  </si>
-  <si>
-    <t>coordinadorregistro1</t>
-  </si>
-  <si>
-    <t>coordinadorregistro1@coordinadorregistro1.com</t>
-  </si>
-  <si>
-    <t>http://evidentia.test/20/profiles/view/7</t>
-  </si>
-  <si>
-    <t>Hart</t>
-  </si>
-  <si>
-    <t>Clara</t>
-  </si>
-  <si>
-    <t>coordinadorregistro2</t>
-  </si>
-  <si>
-    <t>coordinadorregistro2@coordinadorregistro2.com</t>
-  </si>
-  <si>
-    <t>http://evidentia.test/20/profiles/view/8</t>
-  </si>
-  <si>
-    <t>Liu</t>
-  </si>
-  <si>
-    <t>Jamie-Leigh</t>
-  </si>
-  <si>
-    <t>presidente1</t>
-  </si>
-  <si>
-    <t>presidente1@presidente1.com</t>
-  </si>
-  <si>
-    <t>http://evidentia.test/20/profiles/view/9</t>
-  </si>
-  <si>
-    <t>Alé</t>
-  </si>
-  <si>
-    <t>Francisco</t>
-  </si>
-  <si>
-    <t>presidente2</t>
-  </si>
-  <si>
-    <t>presidente2@presidente2.com</t>
-  </si>
-  <si>
-    <t>http://evidentia.test/20/profiles/view/10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -251,28 +268,40 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -562,39 +591,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="17.567139" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="24.708252" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="54.129639" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="49.416504" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="17.567139" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="23.422852" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="34.134521" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="21.137695" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="23.422852" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="23.422852" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="22.280273" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="26.993408" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="23.422852" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="17.567139" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -650,7 +675,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>111111111</v>
       </c>
@@ -663,14 +688,14 @@
       <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
       </c>
       <c r="K2">
         <v>2</v>
@@ -682,27 +707,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>222222222</v>
       </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3">
         <v>2</v>
@@ -714,30 +739,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>333333333</v>
       </c>
       <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>30</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>32</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
         <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
       </c>
       <c r="K4">
         <v>3</v>
@@ -749,206 +774,200 @@
         <v>6.85</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
+        <v>101010101</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>7.85</v>
+      </c>
+      <c r="R5">
+        <v>7.85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>444444444</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
         <v>35</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>36</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" t="s">
         <v>37</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F6" t="s">
         <v>38</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
         <v>39</v>
       </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>555555555</v>
+      </c>
+      <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5">
-        <v>4</v>
-      </c>
-      <c r="R5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6">
-        <v>555555555</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>41</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" t="s">
         <v>42</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E7" t="s">
         <v>43</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F7" t="s">
         <v>44</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>666666666</v>
+      </c>
+      <c r="B8" t="s">
         <v>45</v>
       </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7">
-        <v>666666666</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D8" t="s">
         <v>47</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E8" t="s">
         <v>48</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F8" t="s">
         <v>49</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>777777777</v>
+      </c>
+      <c r="B9" t="s">
         <v>50</v>
       </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="A8">
-        <v>777777777</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
         <v>51</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
         <v>52</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E9" t="s">
         <v>53</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F9" t="s">
         <v>54</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>888888888</v>
+      </c>
+      <c r="B10" t="s">
         <v>55</v>
       </c>
-      <c r="G8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9">
-        <v>888888888</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
         <v>56</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D10" t="s">
         <v>57</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E10" t="s">
         <v>58</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F10" t="s">
         <v>59</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>999999999</v>
+      </c>
+      <c r="B11" t="s">
         <v>60</v>
       </c>
-      <c r="G9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10">
-        <v>999999999</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C11" t="s">
         <v>61</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D11" t="s">
         <v>62</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E11" t="s">
         <v>63</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F11" t="s">
         <v>64</v>
       </c>
-      <c r="F10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="A11">
-        <v>101010101</v>
-      </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" t="s">
-        <v>70</v>
-      </c>
       <c r="G11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11">
-        <v>4</v>
-      </c>
-      <c r="L11">
-        <v>7.85</v>
-      </c>
-      <c r="R11">
-        <v>7.85</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{C2BA17C5-F23F-49B7-9556-CDFED4CA3254}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{88781723-777A-4A4F-BB21-E2708FEEEFB5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solucion de errores de import y correo, ademas de la imagen de inicio
</commit_message>
<xml_diff>
--- a/evidencias2020.xlsx
+++ b/evidencias2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\InnosoftDiploma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fraal\Desktop\InnosoftDiploma-develop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3189A2-40F7-4EDC-AB67-A18C76FB61E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA61E37-1889-48B6-91D2-58E7641B619D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4452" yWindow="2280" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="930" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>alumno2</t>
   </si>
   <si>
-    <t>alumno2@alumno2.com</t>
-  </si>
-  <si>
     <t>http://evidentia.test/20/profiles/view/2</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>secretario1</t>
   </si>
   <si>
-    <t>secretario1@secretario1.com</t>
-  </si>
-  <si>
     <t>http://evidentia.test/20/profiles/view/3</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     <t>secretario2</t>
   </si>
   <si>
-    <t>secretario2@secretario2.com</t>
-  </si>
-  <si>
     <t>http://evidentia.test/20/profiles/view/4</t>
   </si>
   <si>
@@ -237,13 +228,22 @@
     <t>presidente2</t>
   </si>
   <si>
-    <t>presidente2@presidente2.com</t>
-  </si>
-  <si>
     <t>http://evidentia.test/20/profiles/view/10</t>
   </si>
   <si>
-    <t>alumno1@alumno1.com</t>
+    <t>migyanari@alum.us.es</t>
+  </si>
+  <si>
+    <t>enrmerver@alum.us.es</t>
+  </si>
+  <si>
+    <t>pedbiefre@alum.us.es</t>
+  </si>
+  <si>
+    <t>josgatfer@alum.us.es</t>
+  </si>
+  <si>
+    <t>curalepal@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -595,31 +595,31 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="27" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -675,7 +675,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>111111111</v>
       </c>
@@ -689,7 +689,7 @@
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
         <v>21</v>
@@ -707,7 +707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>222222222</v>
       </c>
@@ -721,10 +721,10 @@
         <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" t="s">
         <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
       </c>
       <c r="G3" t="s">
         <v>22</v>
@@ -739,30 +739,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>333333333</v>
       </c>
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" t="s">
         <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K4">
         <v>3</v>
@@ -774,24 +774,24 @@
         <v>6.85</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>101010101</v>
       </c>
       <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" t="s">
         <v>65</v>
-      </c>
-      <c r="C5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" t="s">
-        <v>69</v>
       </c>
       <c r="G5" t="s">
         <v>22</v>
@@ -806,30 +806,30 @@
         <v>7.85</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>444444444</v>
       </c>
       <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" t="s">
         <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
       </c>
       <c r="G6" t="s">
         <v>22</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K6">
         <v>2</v>
@@ -841,122 +841,122 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>555555555</v>
       </c>
       <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
         <v>40</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
         <v>41</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" t="s">
-        <v>44</v>
       </c>
       <c r="G7" t="s">
         <v>22</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>666666666</v>
       </c>
       <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
         <v>45</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" t="s">
         <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" t="s">
-        <v>49</v>
       </c>
       <c r="G8" t="s">
         <v>22</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>777777777</v>
       </c>
       <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
         <v>50</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
         <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" t="s">
-        <v>54</v>
       </c>
       <c r="G9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>888888888</v>
       </c>
       <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
         <v>55</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
         <v>56</v>
-      </c>
-      <c r="D10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" t="s">
-        <v>59</v>
       </c>
       <c r="G10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>999999999</v>
       </c>
       <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" t="s">
         <v>60</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
         <v>61</v>
-      </c>
-      <c r="D11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" t="s">
-        <v>64</v>
       </c>
       <c r="G11" t="s">
         <v>22</v>
@@ -966,7 +966,10 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{C2BA17C5-F23F-49B7-9556-CDFED4CA3254}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{88781723-777A-4A4F-BB21-E2708FEEEFB5}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{C9AB62F0-FDAA-475D-88FB-443C1F2382DA}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{21B6BCF1-E9AB-4428-B0F9-0F4816E11216}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{70E21DDA-3CAC-4DFE-9A1A-819B512B1FC6}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{947A7629-03A9-4C03-83CA-863EDE48B70B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Elección archivo base para envío correos
Se ha actualizado la función de envío de correos para que podamos elegir el archivo fuente del cual queremos coger los datos para hacer el envío de diplomas por correo.
</commit_message>
<xml_diff>
--- a/evidencias2020.xlsx
+++ b/evidencias2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fraal\Desktop\InnosoftDiploma-develop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\InnosoftDiploma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA61E37-1889-48B6-91D2-58E7641B619D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D790D3-9032-4BB4-8919-D533CB0286B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="930" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -231,9 +231,6 @@
     <t>http://evidentia.test/20/profiles/view/10</t>
   </si>
   <si>
-    <t>migyanari@alum.us.es</t>
-  </si>
-  <si>
     <t>enrmerver@alum.us.es</t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>curalepal@gmail.com</t>
+  </si>
+  <si>
+    <t>guilosost@alum.us.es</t>
   </si>
 </sst>
 </file>
@@ -595,31 +595,31 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="27" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -675,7 +675,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>111111111</v>
       </c>
@@ -689,7 +689,7 @@
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
         <v>21</v>
@@ -707,7 +707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>222222222</v>
       </c>
@@ -721,7 +721,7 @@
         <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
         <v>26</v>
@@ -739,7 +739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>333333333</v>
       </c>
@@ -753,7 +753,7 @@
         <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" t="s">
         <v>30</v>
@@ -774,7 +774,7 @@
         <v>6.85</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>101010101</v>
       </c>
@@ -788,7 +788,7 @@
         <v>64</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F5" t="s">
         <v>65</v>
@@ -806,7 +806,7 @@
         <v>7.85</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>444444444</v>
       </c>
@@ -820,7 +820,7 @@
         <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F6" t="s">
         <v>35</v>
@@ -841,7 +841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>555555555</v>
       </c>
@@ -867,7 +867,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>666666666</v>
       </c>
@@ -893,7 +893,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>777777777</v>
       </c>
@@ -916,7 +916,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>888888888</v>
       </c>
@@ -939,7 +939,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>999999999</v>
       </c>
@@ -972,5 +972,6 @@
     <hyperlink ref="E6" r:id="rId5" xr:uid="{947A7629-03A9-4C03-83CA-863EDE48B70B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>